<commit_message>
minor typo fixes in ch 4-5, and discussion section added to end of ch 3
</commit_message>
<xml_diff>
--- a/FRAP-analysis-190408.xlsx
+++ b/FRAP-analysis-190408.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lauramaguire/Google Drive/Thesis/Thesis Repository/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB5B3D4-1C10-3A41-8326-F586FA7C3536}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19D5D29-E171-A748-BF2B-B470AA520419}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="7" xr2:uid="{A9073BF0-BA06-8246-BE23-0DC2BC3153F9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="5" xr2:uid="{A9073BF0-BA06-8246-BE23-0DC2BC3153F9}"/>
   </bookViews>
   <sheets>
     <sheet name="List of datasets" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'List of gels'!$A$1:$N$89</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1423" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1429" uniqueCount="290">
   <si>
     <t>Gel type</t>
   </si>
@@ -1054,6 +1053,15 @@
   </si>
   <si>
     <t xml:space="preserve">10 mg/mL </t>
+  </si>
+  <si>
+    <t>KD predict (M)</t>
+  </si>
+  <si>
+    <t>KD predict (uM)</t>
+  </si>
+  <si>
+    <t>assume Nt = 1 mg/mL</t>
   </si>
 </sst>
 </file>
@@ -1209,7 +1217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1306,6 +1314,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -6885,7 +6897,7 @@
         <v>22.884319607715199</v>
       </c>
       <c r="F4" s="19">
-        <f>D4/E4</f>
+        <f t="shared" ref="F4:F9" si="0">D4/E4</f>
         <v>0.60877559096592826</v>
       </c>
       <c r="G4" s="19">
@@ -6912,7 +6924,7 @@
         <v>36.095885683268797</v>
       </c>
       <c r="F5" s="19">
-        <f>D5/E5</f>
+        <f t="shared" si="0"/>
         <v>0.37065280434427089</v>
       </c>
       <c r="G5" s="19">
@@ -6939,7 +6951,7 @@
         <v>46.031094424366202</v>
       </c>
       <c r="F6" s="19">
-        <f>D6/E6</f>
+        <f t="shared" si="0"/>
         <v>0.43935196350832717</v>
       </c>
       <c r="G6" s="19">
@@ -6966,7 +6978,7 @@
         <v>22.326414077468499</v>
       </c>
       <c r="F7" s="19">
-        <f>D7/E7</f>
+        <f t="shared" si="0"/>
         <v>0.55795189052015715</v>
       </c>
       <c r="G7" s="19">
@@ -6993,7 +7005,7 @@
         <v>41.3677583378227</v>
       </c>
       <c r="F8" s="19">
-        <f>D8/E8</f>
+        <f t="shared" si="0"/>
         <v>0.26461234921016369</v>
       </c>
       <c r="G8" s="19">
@@ -7020,7 +7032,7 @@
         <v>70.394190376426295</v>
       </c>
       <c r="F9" s="19">
-        <f>D9/E9</f>
+        <f t="shared" si="0"/>
         <v>0.60198759042068162</v>
       </c>
       <c r="G9" s="19">
@@ -7093,7 +7105,7 @@
         <v>20.183808492096901</v>
       </c>
       <c r="F12" s="19">
-        <f>D12/E12</f>
+        <f t="shared" ref="F12:F19" si="1">D12/E12</f>
         <v>0.36472679696294841</v>
       </c>
       <c r="G12" s="19">
@@ -7120,7 +7132,7 @@
         <v>10.9011360963647</v>
       </c>
       <c r="F13" s="19">
-        <f>D13/E13</f>
+        <f t="shared" si="1"/>
         <v>1.0045183854533497</v>
       </c>
       <c r="G13" s="19">
@@ -7147,7 +7159,7 @@
         <v>44.560245626773103</v>
       </c>
       <c r="F14" s="19">
-        <f>D14/E14</f>
+        <f t="shared" si="1"/>
         <v>0.28684403889044308</v>
       </c>
       <c r="G14" s="19">
@@ -7174,7 +7186,7 @@
         <v>43.183541617449301</v>
       </c>
       <c r="F15" s="19">
-        <f>D15/E15</f>
+        <f t="shared" si="1"/>
         <v>0.23867899468183543</v>
       </c>
       <c r="G15" s="19">
@@ -7201,7 +7213,7 @@
         <v>30.9104011446341</v>
       </c>
       <c r="F16" s="19">
-        <f>D16/E16</f>
+        <f t="shared" si="1"/>
         <v>0.2702371329976847</v>
       </c>
       <c r="G16" s="19">
@@ -7228,7 +7240,7 @@
         <v>42.569398411928901</v>
       </c>
       <c r="F17" s="19">
-        <f>D17/E17</f>
+        <f t="shared" si="1"/>
         <v>0.22078487921957637</v>
       </c>
       <c r="G17" s="19">
@@ -7255,7 +7267,7 @@
         <v>39.711930712395898</v>
       </c>
       <c r="F18" s="19">
-        <f>D18/E18</f>
+        <f t="shared" si="1"/>
         <v>0.6731692392224502</v>
       </c>
       <c r="G18" s="19">
@@ -7282,7 +7294,7 @@
         <v>53.360414862107604</v>
       </c>
       <c r="F19" s="19">
-        <f>D19/E19</f>
+        <f t="shared" si="1"/>
         <v>0.30545577365373805</v>
       </c>
       <c r="G19" s="19">
@@ -7332,7 +7344,7 @@
         <v>29.004986266572899</v>
       </c>
       <c r="F21" s="19">
-        <f>D21/E21</f>
+        <f t="shared" ref="F21:F38" si="2">D21/E21</f>
         <v>0.96243878855704679</v>
       </c>
       <c r="G21" s="19">
@@ -7359,7 +7371,7 @@
         <v>18.146837422999901</v>
       </c>
       <c r="F22" s="19">
-        <f>D22/E22</f>
+        <f t="shared" si="2"/>
         <v>0.1451881227913602</v>
       </c>
       <c r="G22" s="19">
@@ -7386,7 +7398,7 @@
         <v>17.811075266206501</v>
       </c>
       <c r="F23" s="19">
-        <f>D23/E23</f>
+        <f t="shared" si="2"/>
         <v>3.0005267044081834E-2</v>
       </c>
       <c r="G23" s="19">
@@ -7413,7 +7425,7 @@
         <v>26.701718003743199</v>
       </c>
       <c r="F24" s="19">
-        <f>D24/E24</f>
+        <f t="shared" si="2"/>
         <v>1.5570226973613028</v>
       </c>
       <c r="G24" s="19">
@@ -7440,7 +7452,7 @@
         <v>71.213773666190406</v>
       </c>
       <c r="F25" s="19">
-        <f>D25/E25</f>
+        <f t="shared" si="2"/>
         <v>0.96405073143146136</v>
       </c>
       <c r="G25" s="19">
@@ -7467,7 +7479,7 @@
         <v>26.402570800341099</v>
       </c>
       <c r="F26" s="19">
-        <f>D26/E26</f>
+        <f t="shared" si="2"/>
         <v>0.95749146887188352</v>
       </c>
       <c r="G26" s="19">
@@ -7494,7 +7506,7 @@
         <v>126.26430006096</v>
       </c>
       <c r="F27" s="19">
-        <f>D27/E27</f>
+        <f t="shared" si="2"/>
         <v>1.404117603401104</v>
       </c>
       <c r="G27" s="19">
@@ -7521,7 +7533,7 @@
         <v>71.499631169558</v>
       </c>
       <c r="F28" s="19">
-        <f>D28/E28</f>
+        <f t="shared" si="2"/>
         <v>1.0069137256904195</v>
       </c>
       <c r="G28" s="19">
@@ -7548,7 +7560,7 @@
         <v>25.8287038913023</v>
       </c>
       <c r="F29" s="19">
-        <f>D29/E29</f>
+        <f t="shared" si="2"/>
         <v>1.2828262483032118</v>
       </c>
       <c r="G29" s="19">
@@ -7575,7 +7587,7 @@
         <v>68.139648991330205</v>
       </c>
       <c r="F30" s="19">
-        <f>D30/E30</f>
+        <f t="shared" si="2"/>
         <v>1.4692981262965343</v>
       </c>
       <c r="G30" s="19">
@@ -7602,7 +7614,7 @@
         <v>26.520995286782401</v>
       </c>
       <c r="F31" s="19">
-        <f>D31/E31</f>
+        <f t="shared" si="2"/>
         <v>1.0117614108037212</v>
       </c>
       <c r="G31" s="19">
@@ -7629,7 +7641,7 @@
         <v>27.622707706662698</v>
       </c>
       <c r="F32" s="19">
-        <f>D32/E32</f>
+        <f t="shared" si="2"/>
         <v>1.1281598550893877</v>
       </c>
       <c r="G32" s="19">
@@ -7656,7 +7668,7 @@
         <v>61.437581286543498</v>
       </c>
       <c r="F33" s="19">
-        <f>D33/E33</f>
+        <f t="shared" si="2"/>
         <v>1.2172183985133884</v>
       </c>
       <c r="G33" s="19">
@@ -7683,7 +7695,7 @@
         <v>15.207550491225399</v>
       </c>
       <c r="F34" s="19">
-        <f>D34/E34</f>
+        <f t="shared" si="2"/>
         <v>0.71470362157600187</v>
       </c>
       <c r="G34" s="19">
@@ -7710,7 +7722,7 @@
         <v>31.9935373143629</v>
       </c>
       <c r="F35" s="19">
-        <f>D35/E35</f>
+        <f t="shared" si="2"/>
         <v>1.1813003617494651</v>
       </c>
       <c r="G35" s="19">
@@ -7737,7 +7749,7 @@
         <v>15.584490555396</v>
       </c>
       <c r="F36" s="19">
-        <f>D36/E36</f>
+        <f t="shared" si="2"/>
         <v>1.1764208285663489</v>
       </c>
       <c r="G36" s="19">
@@ -7764,7 +7776,7 @@
         <v>44.2171995934142</v>
       </c>
       <c r="F37" s="19">
-        <f>D37/E37</f>
+        <f t="shared" si="2"/>
         <v>0.9224738762852166</v>
       </c>
       <c r="G37" s="19">
@@ -7791,7 +7803,7 @@
         <v>57.944403738835199</v>
       </c>
       <c r="F38" s="19">
-        <f>D38/E38</f>
+        <f t="shared" si="2"/>
         <v>1.429838654159441</v>
       </c>
       <c r="G38" s="19">
@@ -9329,8 +9341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EE29F74-13EB-B64A-A652-3C18F5FB9619}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -9344,7 +9356,8 @@
     <col min="12" max="12" width="10.83203125" style="1"/>
     <col min="13" max="13" width="12.83203125" style="22" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.83203125" style="1"/>
+    <col min="15" max="15" width="13" style="22" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -9356,6 +9369,10 @@
         <v>266</v>
       </c>
       <c r="N1" s="73"/>
+      <c r="O1" s="73" t="s">
+        <v>289</v>
+      </c>
+      <c r="P1" s="73"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" t="s">
@@ -9400,6 +9417,12 @@
       <c r="N2" s="1" t="s">
         <v>261</v>
       </c>
+      <c r="O2" s="22" t="s">
+        <v>287</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="19">
@@ -9451,6 +9474,14 @@
         <f t="shared" ref="N3:N12" si="5">M3*14912</f>
         <v>3.4482959556699617</v>
       </c>
+      <c r="O3" s="22">
+        <f>$B$39*((1/I3)-1)</f>
+        <v>2.3928907351392089E-5</v>
+      </c>
+      <c r="P3" s="1">
+        <f>O3*1000000</f>
+        <v>23.928907351392088</v>
+      </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="19">
@@ -9499,6 +9530,14 @@
         <f t="shared" si="5"/>
         <v>3.5000103552433544</v>
       </c>
+      <c r="O4" s="22">
+        <f t="shared" ref="O4:O14" si="6">$B$39*((1/I4)-1)</f>
+        <v>2.1593653339165519E-5</v>
+      </c>
+      <c r="P4" s="1">
+        <f t="shared" ref="P4:P14" si="7">O4*1000000</f>
+        <v>21.59365333916552</v>
+      </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="19">
@@ -9517,7 +9556,7 @@
         <v>22.884319607715199</v>
       </c>
       <c r="F5" s="19">
-        <f t="shared" ref="F5:F10" si="6">D5/E5</f>
+        <f t="shared" ref="F5:F10" si="8">D5/E5</f>
         <v>0.60877559096592826</v>
       </c>
       <c r="G5" s="19">
@@ -9550,6 +9589,14 @@
         <f t="shared" si="5"/>
         <v>3.016035673469077</v>
       </c>
+      <c r="O5" s="22">
+        <f t="shared" si="6"/>
+        <v>4.6580608755986996E-5</v>
+      </c>
+      <c r="P5" s="1">
+        <f t="shared" si="7"/>
+        <v>46.580608755986994</v>
+      </c>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="19">
@@ -9568,7 +9615,7 @@
         <v>36.095885683268797</v>
       </c>
       <c r="F6" s="19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.37065280434427089</v>
       </c>
       <c r="G6" s="19">
@@ -9601,6 +9648,14 @@
         <f t="shared" si="5"/>
         <v>3.4155729260816785</v>
       </c>
+      <c r="O6" s="22">
+        <f t="shared" si="6"/>
+        <v>2.5443102715177201E-5</v>
+      </c>
+      <c r="P6" s="1">
+        <f t="shared" si="7"/>
+        <v>25.443102715177201</v>
+      </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="19">
@@ -9619,7 +9674,7 @@
         <v>46.031094424366202</v>
       </c>
       <c r="F7" s="19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.43935196350832717</v>
       </c>
       <c r="G7" s="19">
@@ -9652,6 +9707,14 @@
         <f t="shared" si="5"/>
         <v>3.5335999886652369</v>
       </c>
+      <c r="O7" s="22">
+        <f t="shared" si="6"/>
+        <v>2.0113471564860865E-5</v>
+      </c>
+      <c r="P7" s="1">
+        <f t="shared" si="7"/>
+        <v>20.113471564860866</v>
+      </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="19">
@@ -9670,7 +9733,7 @@
         <v>22.326414077468499</v>
       </c>
       <c r="F8" s="19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.55795189052015715</v>
       </c>
       <c r="G8" s="19">
@@ -9703,6 +9766,14 @@
         <f t="shared" si="5"/>
         <v>3.3087453759162337</v>
       </c>
+      <c r="O8" s="22">
+        <f t="shared" si="6"/>
+        <v>3.0594829960019356E-5</v>
+      </c>
+      <c r="P8" s="1">
+        <f t="shared" si="7"/>
+        <v>30.594829960019357</v>
+      </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="19">
@@ -9721,7 +9792,7 @@
         <v>41.3677583378227</v>
       </c>
       <c r="F9" s="19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.26461234921016369</v>
       </c>
       <c r="G9" s="19">
@@ -9754,6 +9825,14 @@
         <f t="shared" si="5"/>
         <v>3.3728872672265724</v>
       </c>
+      <c r="O9" s="22">
+        <f t="shared" si="6"/>
+        <v>2.7462459710162958E-5</v>
+      </c>
+      <c r="P9" s="1">
+        <f t="shared" si="7"/>
+        <v>27.462459710162957</v>
+      </c>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" s="19">
@@ -9772,7 +9851,7 @@
         <v>70.394190376426295</v>
       </c>
       <c r="F10" s="19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.60198759042068162</v>
       </c>
       <c r="G10" s="19">
@@ -9805,6 +9884,14 @@
         <f t="shared" si="5"/>
         <v>2.2502440989191888</v>
       </c>
+      <c r="O10" s="22">
+        <f t="shared" si="6"/>
+        <v>1.0807577509558548E-4</v>
+      </c>
+      <c r="P10" s="1">
+        <f t="shared" si="7"/>
+        <v>108.07577509558547</v>
+      </c>
     </row>
     <row r="11" spans="1:17">
       <c r="A11" s="19">
@@ -9853,6 +9940,14 @@
         <f t="shared" si="5"/>
         <v>3.5640163136342369</v>
       </c>
+      <c r="O11" s="22">
+        <f t="shared" si="6"/>
+        <v>1.8797197956360783E-5</v>
+      </c>
+      <c r="P11" s="1">
+        <f t="shared" si="7"/>
+        <v>18.797197956360783</v>
+      </c>
     </row>
     <row r="12" spans="1:17" s="24" customFormat="1">
       <c r="A12" s="19">
@@ -9901,8 +9996,14 @@
         <f t="shared" si="5"/>
         <v>3.6717101617218697</v>
       </c>
-      <c r="O12" s="21"/>
-      <c r="P12" s="33"/>
+      <c r="O12" s="22">
+        <f t="shared" si="6"/>
+        <v>1.4312023678010293E-5</v>
+      </c>
+      <c r="P12" s="1">
+        <f t="shared" si="7"/>
+        <v>14.312023678010293</v>
+      </c>
       <c r="Q12" s="33"/>
     </row>
     <row r="13" spans="1:17" s="24" customFormat="1">
@@ -9932,11 +10033,11 @@
         <v>0.35668134024120202</v>
       </c>
       <c r="I13" s="2">
-        <f t="shared" ref="I13:I14" si="7">1-H13/G13</f>
+        <f t="shared" ref="I13:I14" si="9">1-H13/G13</f>
         <v>0.80605586472014645</v>
       </c>
       <c r="J13" s="1">
-        <f t="shared" ref="J13:J14" si="8">(D13-(1-I13)*E13)/I13</f>
+        <f t="shared" ref="J13:J14" si="10">(D13-(1-I13)*E13)/I13</f>
         <v>4.276433790825326</v>
       </c>
       <c r="K13" s="1">
@@ -9944,7 +10045,7 @@
         <v>0.30864287224433468</v>
       </c>
       <c r="L13" s="1">
-        <f t="shared" ref="L13:L14" si="9">K13*E13</f>
+        <f t="shared" ref="L13:L14" si="11">K13*E13</f>
         <v>6.229588625830381</v>
       </c>
       <c r="M13" s="22">
@@ -9952,11 +10053,17 @@
         <v>2.4323746283482251E-4</v>
       </c>
       <c r="N13" s="1">
-        <f t="shared" ref="N13:N14" si="10">M13*14912</f>
+        <f t="shared" ref="N13:N14" si="12">M13*14912</f>
         <v>3.6271570457928735</v>
       </c>
-      <c r="O13" s="21"/>
-      <c r="P13" s="33"/>
+      <c r="O13" s="22">
+        <f t="shared" si="6"/>
+        <v>1.6135246859034696E-5</v>
+      </c>
+      <c r="P13" s="1">
+        <f t="shared" si="7"/>
+        <v>16.135246859034694</v>
+      </c>
       <c r="Q13" s="33"/>
     </row>
     <row r="14" spans="1:17" s="24" customFormat="1">
@@ -9986,11 +10093,11 @@
         <v>0.457887359531786</v>
       </c>
       <c r="I14" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.84475103187671186</v>
       </c>
       <c r="J14" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>10.959443849660218</v>
       </c>
       <c r="K14" s="1">
@@ -9998,7 +10105,7 @@
         <v>0.45252892336780487</v>
       </c>
       <c r="L14" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>4.9330793811738332</v>
       </c>
       <c r="M14" s="22">
@@ -10006,11 +10113,17 @@
         <v>2.4956717975348805E-4</v>
       </c>
       <c r="N14" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>3.7215457844840136</v>
       </c>
-      <c r="O14" s="21"/>
-      <c r="P14" s="33"/>
+      <c r="O14" s="22">
+        <f t="shared" si="6"/>
+        <v>1.2324352070112453E-5</v>
+      </c>
+      <c r="P14" s="1">
+        <f t="shared" si="7"/>
+        <v>12.324352070112454</v>
+      </c>
       <c r="Q14" s="33"/>
     </row>
     <row r="15" spans="1:17" s="19" customFormat="1">
@@ -10025,7 +10138,8 @@
       <c r="L15" s="2"/>
       <c r="M15" s="23"/>
       <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="2"/>
     </row>
     <row r="16" spans="1:17" s="19" customFormat="1">
       <c r="A16" s="19" t="s">
@@ -10040,7 +10154,7 @@
         <v>34.70537769200228</v>
       </c>
       <c r="F16" s="2">
-        <f t="shared" ref="F16" si="11">AVERAGE(F3:F12)</f>
+        <f t="shared" ref="F16" si="13">AVERAGE(F3:F12)</f>
         <v>0.49059654110465251</v>
       </c>
       <c r="G16" s="2">
@@ -10063,9 +10177,10 @@
       <c r="L16" s="2"/>
       <c r="M16" s="23"/>
       <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-    </row>
-    <row r="17" spans="1:15" s="19" customFormat="1">
+      <c r="O16" s="23"/>
+      <c r="P16" s="2"/>
+    </row>
+    <row r="17" spans="1:16" s="19" customFormat="1">
       <c r="A17" s="19" t="s">
         <v>241</v>
       </c>
@@ -10078,7 +10193,7 @@
         <v>16.546726043182563</v>
       </c>
       <c r="F17" s="2">
-        <f t="shared" ref="F17" si="12">STDEVA(F3:F12)</f>
+        <f t="shared" ref="F17" si="14">STDEVA(F3:F12)</f>
         <v>0.13480963804884469</v>
       </c>
       <c r="G17" s="2">
@@ -10101,9 +10216,10 @@
       <c r="L17" s="2"/>
       <c r="M17" s="23"/>
       <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-    </row>
-    <row r="18" spans="1:15" s="19" customFormat="1">
+      <c r="O17" s="23"/>
+      <c r="P17" s="2"/>
+    </row>
+    <row r="18" spans="1:16" s="19" customFormat="1">
       <c r="A18" t="s">
         <v>240</v>
       </c>
@@ -10118,7 +10234,7 @@
         <v>4.9890256176398733</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" ref="F18" si="13">F17/SQRT(COUNT(F3:F12)-1)</f>
+        <f t="shared" ref="F18" si="15">F17/SQRT(COUNT(F3:F12)-1)</f>
         <v>5.5035804271492988E-2</v>
       </c>
       <c r="G18" s="1">
@@ -10141,9 +10257,10 @@
       <c r="L18" s="2"/>
       <c r="M18" s="23"/>
       <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-    </row>
-    <row r="19" spans="1:15" s="19" customFormat="1">
+      <c r="O18" s="23"/>
+      <c r="P18" s="2"/>
+    </row>
+    <row r="19" spans="1:16" s="19" customFormat="1">
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -10155,9 +10272,10 @@
       <c r="L19" s="2"/>
       <c r="M19" s="23"/>
       <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-    </row>
-    <row r="20" spans="1:15" s="19" customFormat="1">
+      <c r="O19" s="23"/>
+      <c r="P19" s="2"/>
+    </row>
+    <row r="20" spans="1:16" s="19" customFormat="1">
       <c r="A20" s="20" t="s">
         <v>260</v>
       </c>
@@ -10175,9 +10293,10 @@
       <c r="L20" s="2"/>
       <c r="M20" s="23"/>
       <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-    </row>
-    <row r="21" spans="1:15" s="19" customFormat="1">
+      <c r="O20" s="23"/>
+      <c r="P20" s="2"/>
+    </row>
+    <row r="21" spans="1:16" s="19" customFormat="1">
       <c r="A21" s="20" t="s">
         <v>259</v>
       </c>
@@ -10196,9 +10315,10 @@
       <c r="L21" s="2"/>
       <c r="M21" s="23"/>
       <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-    </row>
-    <row r="22" spans="1:15" s="19" customFormat="1">
+      <c r="O21" s="23"/>
+      <c r="P21" s="2"/>
+    </row>
+    <row r="22" spans="1:16" s="19" customFormat="1">
       <c r="A22" s="20" t="s">
         <v>258</v>
       </c>
@@ -10216,9 +10336,10 @@
       <c r="L22" s="2"/>
       <c r="M22" s="23"/>
       <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-    </row>
-    <row r="23" spans="1:15">
+      <c r="O22" s="23"/>
+      <c r="P22" s="2"/>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23" s="20" t="s">
         <v>257</v>
       </c>
@@ -10226,7 +10347,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:16">
       <c r="A24" s="20" t="s">
         <v>256</v>
       </c>
@@ -10235,7 +10356,7 @@
         <v>5.4500000000000002E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:16">
       <c r="A25" s="20" t="s">
         <v>255</v>
       </c>
@@ -10244,7 +10365,7 @@
         <v>3.9500000000000001E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:16">
       <c r="A26" s="20" t="s">
         <v>254</v>
       </c>
@@ -10252,7 +10373,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:16">
       <c r="A28" t="s">
         <v>253</v>
       </c>
@@ -10261,7 +10382,7 @@
         <v>545000</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:16">
       <c r="A29" t="s">
         <v>252</v>
       </c>
@@ -10270,7 +10391,7 @@
         <v>395000</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:16">
       <c r="A30" t="s">
         <v>251</v>
       </c>
@@ -10279,7 +10400,7 @@
         <v>4.9600000000000001E-8</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:16">
       <c r="A31" t="s">
         <v>250</v>
       </c>
@@ -10342,9 +10463,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -11198,8 +11320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A544C46-8A4E-704E-9B4C-D59AC133C1EF}">
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3:L9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11212,6 +11334,8 @@
     <col min="12" max="12" width="10.83203125" style="1"/>
     <col min="13" max="13" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -11223,6 +11347,10 @@
         <v>266</v>
       </c>
       <c r="N1" s="72"/>
+      <c r="O1" s="75" t="s">
+        <v>289</v>
+      </c>
+      <c r="P1" s="75"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" t="s">
@@ -11267,6 +11395,12 @@
       <c r="N2" s="1" t="s">
         <v>261</v>
       </c>
+      <c r="O2" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="19">
@@ -11318,8 +11452,14 @@
         <f t="shared" ref="N3:N11" si="4">M3*14912</f>
         <v>2.5891214415695858</v>
       </c>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
+      <c r="O3" s="19">
+        <f>'CCT1'!$B$39*((1/'CCT2'!I3)-1)</f>
+        <v>1.8441231456248124E-5</v>
+      </c>
+      <c r="P3" s="2">
+        <f>O3*1000000</f>
+        <v>18.441231456248126</v>
+      </c>
       <c r="Q3" s="19"/>
     </row>
     <row r="4" spans="1:17">
@@ -11372,8 +11512,14 @@
         <f t="shared" si="4"/>
         <v>2.5539537432681247</v>
       </c>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
+      <c r="O4" s="19">
+        <f>'CCT1'!$B$39*((1/'CCT2'!I4)-1)</f>
+        <v>2.0541987357512104E-5</v>
+      </c>
+      <c r="P4" s="2">
+        <f t="shared" ref="P4:P12" si="5">O4*1000000</f>
+        <v>20.541987357512102</v>
+      </c>
       <c r="Q4" s="19"/>
     </row>
     <row r="5" spans="1:17">
@@ -11426,8 +11572,14 @@
         <f t="shared" si="4"/>
         <v>2.6978206299819663</v>
       </c>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
+      <c r="O5" s="19">
+        <f>'CCT1'!$B$39*((1/'CCT2'!I5)-1)</f>
+        <v>1.2294306594381669E-5</v>
+      </c>
+      <c r="P5" s="2">
+        <f t="shared" si="5"/>
+        <v>12.29430659438167</v>
+      </c>
       <c r="Q5" s="19"/>
     </row>
     <row r="6" spans="1:17">
@@ -11480,8 +11632,14 @@
         <f t="shared" si="4"/>
         <v>2.7040864792381698</v>
       </c>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
+      <c r="O6" s="19">
+        <f>'CCT1'!$B$39*((1/'CCT2'!I6)-1)</f>
+        <v>1.1955038210475269E-5</v>
+      </c>
+      <c r="P6" s="2">
+        <f t="shared" si="5"/>
+        <v>11.955038210475269</v>
+      </c>
       <c r="Q6" s="19"/>
     </row>
     <row r="7" spans="1:17">
@@ -11534,8 +11692,14 @@
         <f t="shared" si="4"/>
         <v>2.5110867667087438</v>
       </c>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
+      <c r="O7" s="19">
+        <f>'CCT1'!$B$39*((1/'CCT2'!I7)-1)</f>
+        <v>2.3182238277439123E-5</v>
+      </c>
+      <c r="P7" s="2">
+        <f t="shared" si="5"/>
+        <v>23.182238277439122</v>
+      </c>
       <c r="Q7" s="19"/>
     </row>
     <row r="8" spans="1:17">
@@ -11588,228 +11752,258 @@
         <f t="shared" si="4"/>
         <v>2.5225490412151976</v>
       </c>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19"/>
+      <c r="O8" s="19">
+        <f>'CCT1'!$B$39*((1/'CCT2'!I8)-1)</f>
+        <v>2.246746787102536E-5</v>
+      </c>
+      <c r="P8" s="2">
+        <f t="shared" si="5"/>
+        <v>22.467467871025359</v>
+      </c>
       <c r="Q8" s="19"/>
     </row>
-    <row r="9" spans="1:17" s="24" customFormat="1">
-      <c r="A9" s="19">
+    <row r="9" spans="1:17" s="33" customFormat="1">
+      <c r="A9" s="20">
         <v>35</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="20" t="s">
         <v>270</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="20" t="s">
         <v>212</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="20">
         <v>5.8842396681164404</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="20">
         <v>34.9883130236109</v>
       </c>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19">
+      <c r="F9" s="20"/>
+      <c r="G9" s="20">
         <v>2.7798993676274999</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H9" s="20">
         <v>0.56505400079923995</v>
       </c>
-      <c r="I9" s="25">
+      <c r="I9" s="21">
         <f t="shared" si="1"/>
         <v>0.79673580728158366</v>
       </c>
-      <c r="J9" s="26">
+      <c r="J9" s="31">
         <f t="shared" si="2"/>
         <v>-1.540826359236557</v>
       </c>
-      <c r="K9" s="26">
+      <c r="K9" s="31">
         <f>1/(1+3*E9/'CCT1'!$B$36)</f>
         <v>0.27182995762976481</v>
       </c>
-      <c r="L9" s="25">
+      <c r="L9" s="21">
         <f t="shared" si="3"/>
         <v>9.5108716467450982</v>
       </c>
-      <c r="M9" s="27">
+      <c r="M9" s="32">
         <f>'CCT1'!$B$25*I9/(I9+1)</f>
         <v>1.7515688316602031E-4</v>
       </c>
-      <c r="N9" s="26">
+      <c r="N9" s="31">
         <f t="shared" si="4"/>
         <v>2.6119394417716948</v>
       </c>
-      <c r="O9" s="28"/>
-      <c r="P9" s="28"/>
-      <c r="Q9" s="28"/>
-    </row>
-    <row r="10" spans="1:17">
-      <c r="A10" s="19">
+      <c r="O9" s="19">
+        <f>'CCT1'!$B$39*((1/'CCT2'!I9)-1)</f>
+        <v>1.7108449358859719E-5</v>
+      </c>
+      <c r="P9" s="2">
+        <f t="shared" si="5"/>
+        <v>17.108449358859719</v>
+      </c>
+      <c r="Q9" s="20"/>
+    </row>
+    <row r="10" spans="1:17" s="24" customFormat="1">
+      <c r="A10" s="28">
         <v>37</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="28" t="s">
         <v>212</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="28">
         <v>27.915523844514201</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="28">
         <v>29.004986266572899</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="28">
         <f>D10/E10</f>
         <v>0.96243878855704679</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="28">
         <v>3.4853884344771</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="28">
         <v>0.40756119279391001</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="25">
         <f t="shared" si="1"/>
         <v>0.88306577575045664</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="26">
         <f t="shared" si="2"/>
         <v>27.77125889090506</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="26">
         <f>1/(1+3*E10/'CCT1'!$B$36)</f>
         <v>0.3104938453746367</v>
       </c>
-      <c r="L10" s="2">
+      <c r="L10" s="25">
         <f t="shared" si="3"/>
         <v>9.0058697209467464</v>
       </c>
-      <c r="M10" s="22">
+      <c r="M10" s="27">
         <f>'CCT1'!$B$25*I10/(I10+1)</f>
         <v>1.8523568635430115E-4</v>
       </c>
-      <c r="N10" s="1">
+      <c r="N10" s="26">
         <f t="shared" si="4"/>
         <v>2.7622345549153389</v>
       </c>
-      <c r="O10" t="s">
+      <c r="O10" s="19">
+        <f>'CCT1'!$B$39*((1/'CCT2'!I10)-1)</f>
+        <v>8.8799943682369469E-6</v>
+      </c>
+      <c r="P10" s="2">
+        <f t="shared" si="5"/>
+        <v>8.8799943682369467</v>
+      </c>
+      <c r="Q10" s="24" t="s">
         <v>284</v>
       </c>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
-    </row>
-    <row r="11" spans="1:17">
-      <c r="A11" s="19">
+    </row>
+    <row r="11" spans="1:17" s="24" customFormat="1">
+      <c r="A11" s="28">
         <v>40</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="28" t="s">
         <v>212</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="28">
         <v>2.6347052600453602</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="28">
         <v>18.146837422999901</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="28">
         <f>D11/E11</f>
         <v>0.1451881227913602</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="28">
         <v>4.7232539722014604</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="28">
         <v>0.54556938448958903</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="25">
         <f t="shared" si="1"/>
         <v>0.8844928966978024</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="26">
         <f t="shared" si="2"/>
         <v>0.6089552976961331</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11" s="26">
         <f>1/(1+3*E11/'CCT1'!$B$36)</f>
         <v>0.41852287451621084</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L11" s="25">
         <f t="shared" si="3"/>
         <v>7.5948665616522666</v>
       </c>
-      <c r="M11" s="22">
+      <c r="M11" s="27">
         <f>'CCT1'!$B$25*I11/(I11+1)</f>
         <v>1.8539454025421977E-4</v>
       </c>
-      <c r="N11" s="1">
+      <c r="N11" s="26">
         <f t="shared" si="4"/>
         <v>2.7646033842709254</v>
       </c>
-      <c r="O11" t="s">
+      <c r="O11" s="19">
+        <f>'CCT1'!$B$39*((1/'CCT2'!I11)-1)</f>
+        <v>8.7574657650016922E-6</v>
+      </c>
+      <c r="P11" s="2">
+        <f t="shared" si="5"/>
+        <v>8.757465765001692</v>
+      </c>
+      <c r="Q11" s="24" t="s">
         <v>284</v>
       </c>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
-    </row>
-    <row r="12" spans="1:17">
-      <c r="A12" s="19">
+    </row>
+    <row r="12" spans="1:17" s="24" customFormat="1">
+      <c r="A12" s="28">
         <v>43</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="28" t="s">
         <v>213</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="28" t="s">
         <v>212</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="28">
         <v>0.53442606970476703</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E12" s="28">
         <v>17.811075266206501</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F12" s="28">
         <f>D12/E12</f>
         <v>3.0005267044081834E-2</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="28">
         <v>5.0177195148059202</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="28">
         <v>0.63146230944061599</v>
       </c>
-      <c r="I12" s="2">
-        <f t="shared" ref="I12" si="5">1-H12/G12</f>
+      <c r="I12" s="25">
+        <f t="shared" ref="I12" si="6">1-H12/G12</f>
         <v>0.87415352580443306</v>
       </c>
-      <c r="J12" s="1">
-        <f t="shared" ref="J12" si="6">(D12-(1-I12)*E12)/I12</f>
+      <c r="J12" s="26">
+        <f t="shared" ref="J12" si="7">(D12-(1-I12)*E12)/I12</f>
         <v>-1.952786214078704</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="26">
         <f>1/(1+3*E12/'CCT1'!$B$36)</f>
         <v>0.42307464580291987</v>
       </c>
-      <c r="L12" s="2">
-        <f t="shared" ref="L12" si="7">K12*E12</f>
+      <c r="L12" s="25">
+        <f t="shared" ref="L12" si="8">K12*E12</f>
         <v>7.5354143596194625</v>
       </c>
-      <c r="M12" s="22">
+      <c r="M12" s="27">
         <f>'CCT1'!$B$25*I12/(I12+1)</f>
         <v>1.8423818429951931E-4</v>
       </c>
-      <c r="N12" s="1">
-        <f t="shared" ref="N12" si="8">M12*14912</f>
+      <c r="N12" s="26">
+        <f t="shared" ref="N12" si="9">M12*14912</f>
         <v>2.7473598042744318</v>
       </c>
-      <c r="O12" s="37" t="s">
+      <c r="O12" s="19">
+        <f>'CCT1'!$B$39*((1/'CCT2'!I12)-1)</f>
+        <v>9.65422561678855E-6</v>
+      </c>
+      <c r="P12" s="2">
+        <f t="shared" si="5"/>
+        <v>9.6542256167885494</v>
+      </c>
+      <c r="Q12" s="74" t="s">
         <v>284</v>
       </c>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="19"/>
     </row>
     <row r="13" spans="1:17">
       <c r="A13" s="19"/>
@@ -11827,7 +12021,7 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="19"/>
-      <c r="P13" s="19"/>
+      <c r="P13" s="2"/>
       <c r="Q13" s="19"/>
     </row>
     <row r="14" spans="1:17">
@@ -11837,27 +12031,27 @@
       <c r="B14" s="19"/>
       <c r="C14" s="19"/>
       <c r="D14" s="2">
-        <f t="shared" ref="D14:I14" si="9">AVERAGE(D3:D9)</f>
+        <f t="shared" ref="D14:I14" si="10">AVERAGE(D3:D9)</f>
         <v>12.822428494224852</v>
       </c>
       <c r="E14" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>41.326320771271405</v>
       </c>
       <c r="F14" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.33252834311095464</v>
       </c>
       <c r="G14" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3.1442735107485187</v>
       </c>
       <c r="H14" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.64222142154123518</v>
       </c>
       <c r="I14" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.79035511101129763</v>
       </c>
       <c r="J14" s="2">
@@ -11865,11 +12059,11 @@
         <v>5.2242409632684588</v>
       </c>
       <c r="K14" s="2">
-        <f t="shared" ref="K14:L14" si="10">AVERAGE(K3:K9)</f>
+        <f t="shared" ref="K14:L14" si="11">AVERAGE(K3:K9)</f>
         <v>0.24381343070363798</v>
       </c>
       <c r="L14" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9.8768048437695519</v>
       </c>
       <c r="M14" s="2" t="s">
@@ -11877,7 +12071,7 @@
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="19"/>
-      <c r="P14" s="19"/>
+      <c r="P14" s="2"/>
       <c r="Q14" s="19"/>
     </row>
     <row r="15" spans="1:17">
@@ -11887,27 +12081,27 @@
       <c r="B15" s="19"/>
       <c r="C15" s="19"/>
       <c r="D15" s="2">
-        <f t="shared" ref="D15:I15" si="11">STDEVA(D3:D9)</f>
+        <f t="shared" ref="D15:I15" si="12">STDEVA(D3:D9)</f>
         <v>6.9731889016687632</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>7.2057868063392618</v>
       </c>
       <c r="F15" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.16972371463832647</v>
       </c>
       <c r="G15" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.60343176745670168</v>
       </c>
       <c r="H15" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>7.9487171526184133E-2</v>
       </c>
       <c r="I15" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>4.2877750625749327E-2</v>
       </c>
       <c r="J15" s="2">
@@ -11915,17 +12109,17 @@
         <v>7.827543083818524</v>
       </c>
       <c r="K15" s="2">
-        <f t="shared" ref="K15:L15" si="12">STDEVA(K3:K9)</f>
+        <f t="shared" ref="K15:L15" si="13">STDEVA(K3:K9)</f>
         <v>3.2573484552006871E-2</v>
       </c>
       <c r="L15" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.42545313956194941</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="19"/>
-      <c r="P15" s="19"/>
+      <c r="P15" s="2"/>
       <c r="Q15" s="19"/>
     </row>
     <row r="16" spans="1:17">
@@ -11933,27 +12127,27 @@
         <v>240</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" ref="D16:I16" si="13">D15/SQRT(COUNT(D3:D9)-1)</f>
+        <f t="shared" ref="D16:I16" si="14">D15/SQRT(COUNT(D3:D9)-1)</f>
         <v>2.8467924481878555</v>
       </c>
       <c r="E16" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.9417501451350629</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>7.5902752665014825E-2</v>
       </c>
       <c r="G16" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.24634998747578582</v>
       </c>
       <c r="H16" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3.2450501889372527E-2</v>
       </c>
       <c r="I16" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.7504768391897997E-2</v>
       </c>
       <c r="J16" s="1">
@@ -11961,11 +12155,11 @@
         <v>3.195581082501147</v>
       </c>
       <c r="K16" s="1">
-        <f t="shared" ref="K16:L16" si="14">K15/SQRT(COUNT(K3:K9)-1)</f>
+        <f t="shared" ref="K16:L16" si="15">K15/SQRT(COUNT(K3:K9)-1)</f>
         <v>1.3298069382807857E-2</v>
       </c>
       <c r="L16" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.1736905168986492</v>
       </c>
     </row>
@@ -11978,35 +12172,35 @@
         <v>10.361551724754777</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" ref="E18:L18" si="15">AVERAGE(E10:E12)</f>
+        <f t="shared" ref="E18:L18" si="16">AVERAGE(E10:E12)</f>
         <v>21.654299651926436</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.37921072613082957</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>4.4087873071614938</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.52819762890803834</v>
       </c>
       <c r="I18" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.88057073275089737</v>
       </c>
       <c r="J18" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8.8091426581741636</v>
       </c>
       <c r="K18" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.38403045523125573</v>
       </c>
       <c r="L18" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8.0453835474061588</v>
       </c>
     </row>
@@ -12016,35 +12210,35 @@
         <v>15.238413501913934</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" ref="E19:L19" si="16">STDEVA(E10:E12)</f>
+        <f t="shared" ref="E19:L19" si="17">STDEVA(E10:E12)</f>
         <v>6.3680946394145694</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.50836306137012366</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.8131276637167385</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.11295689854054647</v>
       </c>
       <c r="I19" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>5.6030864079452281E-3</v>
       </c>
       <c r="J19" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>16.471551806402001</v>
       </c>
       <c r="K19" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>6.3725225753739914E-2</v>
       </c>
       <c r="L19" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.83233641531151192</v>
       </c>
     </row>
@@ -12054,42 +12248,43 @@
         <v>8.797902137352839</v>
       </c>
       <c r="E20" s="1">
-        <f t="shared" ref="E20:L20" si="17">E19/SQRT(COUNT(E10:E12))</f>
+        <f t="shared" ref="E20:L20" si="18">E19/SQRT(COUNT(E10:E12))</f>
         <v>3.6766211542910145</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.29350355032810316</v>
       </c>
       <c r="G20" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.46945947553239048</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>6.5215695779209756E-2</v>
       </c>
       <c r="I20" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>3.2349434459199109E-3</v>
       </c>
       <c r="J20" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>9.5098548693970617</v>
       </c>
       <c r="K20" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>3.6791776243091413E-2</v>
       </c>
       <c r="L20" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.48054965343642958</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="K1:L1"/>
+    <mergeCell ref="O1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
working through ch 4 edits, very rough draft fluorimetry discussion
</commit_message>
<xml_diff>
--- a/FRAP-analysis-190408.xlsx
+++ b/FRAP-analysis-190408.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lauramaguire/Google Drive/Thesis/Thesis Repository/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19D5D29-E171-A748-BF2B-B470AA520419}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC730963-066B-F144-B058-57D9225C3A6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="5" xr2:uid="{A9073BF0-BA06-8246-BE23-0DC2BC3153F9}"/>
   </bookViews>
@@ -9342,7 +9342,7 @@
   <dimension ref="A1:Q39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -10178,7 +10178,10 @@
       <c r="M16" s="23"/>
       <c r="N16" s="2"/>
       <c r="O16" s="23"/>
-      <c r="P16" s="2"/>
+      <c r="P16" s="2">
+        <f>AVERAGE(P3:P14)</f>
+        <v>30.446802421322388</v>
+      </c>
     </row>
     <row r="17" spans="1:16" s="19" customFormat="1">
       <c r="A17" s="19" t="s">
@@ -10217,7 +10220,10 @@
       <c r="M17" s="23"/>
       <c r="N17" s="2"/>
       <c r="O17" s="23"/>
-      <c r="P17" s="2"/>
+      <c r="P17" s="2">
+        <f>STDEVA(P3:P14)</f>
+        <v>26.072363389155459</v>
+      </c>
     </row>
     <row r="18" spans="1:16" s="19" customFormat="1">
       <c r="A18" t="s">
@@ -10253,12 +10259,30 @@
         <f>J17/SQRT(COUNT(J3:J14)-1)</f>
         <v>2.2671449439466147</v>
       </c>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="23"/>
-      <c r="P18" s="2"/>
+      <c r="K18" s="1">
+        <f t="shared" ref="K18:P18" si="16">K17/SQRT(COUNT(K3:K14)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="L18" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="M18" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="N18" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="O18" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="P18" s="1">
+        <f t="shared" si="16"/>
+        <v>7.8611133417843204</v>
+      </c>
     </row>
     <row r="19" spans="1:16" s="19" customFormat="1">
       <c r="D19" s="2"/>
@@ -11321,7 +11345,7 @@
   <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:P1"/>
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -12071,7 +12095,10 @@
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="19"/>
-      <c r="P14" s="2"/>
+      <c r="P14" s="2">
+        <f>AVERAGE(P3:P9)</f>
+        <v>17.998674160848768</v>
+      </c>
       <c r="Q14" s="19"/>
     </row>
     <row r="15" spans="1:17">
@@ -12116,10 +12143,22 @@
         <f t="shared" si="13"/>
         <v>0.42545313956194941</v>
       </c>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="19"/>
-      <c r="P15" s="2"/>
+      <c r="M15" s="2">
+        <f t="shared" ref="M15:P15" si="14">STDEVA(M3:M9)</f>
+        <v>5.2429593964449745E-6</v>
+      </c>
+      <c r="N15" s="2">
+        <f t="shared" si="14"/>
+        <v>7.8183010519787557E-2</v>
+      </c>
+      <c r="O15" s="2">
+        <f t="shared" si="14"/>
+        <v>4.5343429914199493E-6</v>
+      </c>
+      <c r="P15" s="2">
+        <f t="shared" si="14"/>
+        <v>4.5343429914199413</v>
+      </c>
       <c r="Q15" s="19"/>
     </row>
     <row r="16" spans="1:17">
@@ -12127,27 +12166,27 @@
         <v>240</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" ref="D16:I16" si="14">D15/SQRT(COUNT(D3:D9)-1)</f>
+        <f t="shared" ref="D16:I16" si="15">D15/SQRT(COUNT(D3:D9)-1)</f>
         <v>2.8467924481878555</v>
       </c>
       <c r="E16" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2.9417501451350629</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>7.5902752665014825E-2</v>
       </c>
       <c r="G16" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.24634998747578582</v>
       </c>
       <c r="H16" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>3.2450501889372527E-2</v>
       </c>
       <c r="I16" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.7504768391897997E-2</v>
       </c>
       <c r="J16" s="1">
@@ -12155,12 +12194,28 @@
         <v>3.195581082501147</v>
       </c>
       <c r="K16" s="1">
-        <f t="shared" ref="K16:L16" si="15">K15/SQRT(COUNT(K3:K9)-1)</f>
+        <f t="shared" ref="K16:L16" si="16">K15/SQRT(COUNT(K3:K9)-1)</f>
         <v>1.3298069382807857E-2</v>
       </c>
       <c r="L16" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.1736905168986492</v>
+      </c>
+      <c r="M16" s="1">
+        <f t="shared" ref="M16:P16" si="17">M15/SQRT(COUNT(M3:M9)-1)</f>
+        <v>2.140429210570108E-6</v>
+      </c>
+      <c r="N16" s="1">
+        <f t="shared" si="17"/>
+        <v>3.1918080388021491E-2</v>
+      </c>
+      <c r="O16" s="1">
+        <f t="shared" si="17"/>
+        <v>1.8511377746239933E-6</v>
+      </c>
+      <c r="P16" s="1">
+        <f t="shared" si="17"/>
+        <v>1.8511377746239899</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -12172,35 +12227,35 @@
         <v>10.361551724754777</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" ref="E18:L18" si="16">AVERAGE(E10:E12)</f>
+        <f t="shared" ref="E18:L18" si="18">AVERAGE(E10:E12)</f>
         <v>21.654299651926436</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.37921072613082957</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>4.4087873071614938</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.52819762890803834</v>
       </c>
       <c r="I18" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.88057073275089737</v>
       </c>
       <c r="J18" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>8.8091426581741636</v>
       </c>
       <c r="K18" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.38403045523125573</v>
       </c>
       <c r="L18" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>8.0453835474061588</v>
       </c>
     </row>
@@ -12210,35 +12265,35 @@
         <v>15.238413501913934</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" ref="E19:L19" si="17">STDEVA(E10:E12)</f>
+        <f t="shared" ref="E19:L19" si="19">STDEVA(E10:E12)</f>
         <v>6.3680946394145694</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.50836306137012366</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.8131276637167385</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.11295689854054647</v>
       </c>
       <c r="I19" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>5.6030864079452281E-3</v>
       </c>
       <c r="J19" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>16.471551806402001</v>
       </c>
       <c r="K19" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>6.3725225753739914E-2</v>
       </c>
       <c r="L19" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.83233641531151192</v>
       </c>
     </row>
@@ -12248,35 +12303,35 @@
         <v>8.797902137352839</v>
       </c>
       <c r="E20" s="1">
-        <f t="shared" ref="E20:L20" si="18">E19/SQRT(COUNT(E10:E12))</f>
+        <f t="shared" ref="E20:L20" si="20">E19/SQRT(COUNT(E10:E12))</f>
         <v>3.6766211542910145</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0.29350355032810316</v>
       </c>
       <c r="G20" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0.46945947553239048</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>6.5215695779209756E-2</v>
       </c>
       <c r="I20" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>3.2349434459199109E-3</v>
       </c>
       <c r="J20" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>9.5098548693970617</v>
       </c>
       <c r="K20" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>3.6791776243091413E-2</v>
       </c>
       <c r="L20" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0.48054965343642958</v>
       </c>
     </row>

</xml_diff>